<commit_message>
run   many scenario   ====> using   or
</commit_message>
<xml_diff>
--- a/resources/testData/TestData.xlsx
+++ b/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{330F5E6A-BDBB-4409-BF09-F10F1F0D34EE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{ADCC27F9-70FF-4385-95CD-6602DEDF8265}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="20" firstSheet="15" tabRatio="729" windowHeight="13140" windowWidth="24240" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView tabRatio="729" windowHeight="13140" windowWidth="24240" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Input" r:id="rId1" sheetId="1"/>
@@ -28,19 +28,18 @@
     <sheet name="EnqueteClient" r:id="rId18" sheetId="16"/>
     <sheet name="EnquetePersonnel" r:id="rId19" sheetId="17"/>
     <sheet name="IncidentEnv" r:id="rId20" sheetId="18"/>
-    <sheet name="EvaluationAspect" r:id="rId21" sheetId="28"/>
-    <sheet name="IncidentSec" r:id="rId22" sheetId="19"/>
-    <sheet name="ModuleVendu" r:id="rId23" sheetId="20"/>
-    <sheet name="RisqueOpp" r:id="rId24" sheetId="23"/>
-    <sheet name="JourConge" r:id="rId25" sheetId="24"/>
-    <sheet name="SommeAgenda" r:id="rId26" sheetId="25"/>
+    <sheet name="IncidentSec" r:id="rId21" sheetId="19"/>
+    <sheet name="ModuleVendu" r:id="rId22" sheetId="20"/>
+    <sheet name="RisqueOpp" r:id="rId23" sheetId="23"/>
+    <sheet name="JourConge" r:id="rId24" sheetId="24"/>
+    <sheet name="SommeAgenda" r:id="rId25" sheetId="25"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="521">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1037,6 +1036,9 @@
     <t>AUDIT</t>
   </si>
   <si>
+    <t>AUTO</t>
+  </si>
+  <si>
     <t>09/17/2020</t>
   </si>
   <si>
@@ -1541,6 +1543,30 @@
     <t>sana</t>
   </si>
   <si>
+    <t>Type de thème 2021-06-01T11:39:00.018512100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> formation auto2021-06-01T11:39:14.345584700</t>
+  </si>
+  <si>
+    <t>SOCIETE AUTO2021-06-01T11:39:25.383552700</t>
+  </si>
+  <si>
+    <t>Type de critére2021-06-01T11:39:39.468828300</t>
+  </si>
+  <si>
+    <t>Théme AUTO2021-06-01T11:39:53.533063400</t>
+  </si>
+  <si>
+    <t>ORGANISME AUTO2021-06-01T11:40:06.644488300</t>
+  </si>
+  <si>
+    <t>Type de thème 2021-06-01T11:52:43.031927700</t>
+  </si>
+  <si>
+    <t>Type de thème 2021-06-01T14:15:19.935951900</t>
+  </si>
+  <si>
     <t>2021-06-02T10:13:56.685749800</t>
   </si>
   <si>
@@ -1559,37 +1585,52 @@
     <t>ORGANISME AUTO2021-06-02T10:15:02.973214</t>
   </si>
   <si>
-    <t>Aspect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facteur AUTO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facteur </t>
-  </si>
-  <si>
-    <t>Activité/Service</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            Aspect AUTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieu AUTO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition AUTO </t>
-  </si>
-  <si>
-    <t>2021-06-04T10:32:42.698874100</t>
-  </si>
-  <si>
-    <t>2021-06-04T11:28:56.958915200</t>
-  </si>
-  <si>
-    <t>2021-06-04T11:28:59.222325700</t>
+    <t>Source Action Auto2021-06-03T15:57:02.582</t>
+  </si>
+  <si>
+    <t>Type Action Auto 2021-06-03T15:57:11.536</t>
+  </si>
+  <si>
+    <t>Source Action Auto2021-06-04T08:39:51.545</t>
+  </si>
+  <si>
+    <t>Type Action Auto 2021-06-04T08:40:00.185</t>
+  </si>
+  <si>
+    <t>désignation  action  simplifie  vz7w4dNWNeS 7e4QOsl0RPu Fb90QOB8LL3 kI47yG878eK wsytWdKVXct wE1D83UdQVF 3xzGBkfu375 Z28A6G7dRHP PuX26D07V8O Y4Gokujj0Eq HVKX5D3UUmH</t>
+  </si>
+  <si>
+    <t>Znf7FSmVew</t>
+  </si>
+  <si>
+    <t>désignation  action  simplifie  siOusjpmQrG 66MJxTpJE09 gmGpWfxEStx zhg6wbjnYRh h92BYRC4G0R evMduSaX6eB 4xUlCWQ824E YhobK8rLWXi 5P47P8O8Yk9 ry23sZ6lspE YDObJCwyzi7</t>
+  </si>
+  <si>
+    <t>GdO6c5TAQl</t>
+  </si>
+  <si>
+    <t>Source Action Auto2021-06-04T11:20:49.170</t>
+  </si>
+  <si>
+    <t>Type Action Auto 2021-06-04T11:20:58.106</t>
+  </si>
+  <si>
+    <t>désignation  action  simplifie  vMrJHSotBVI 683Wk0lIMu8 7NUQOpq0tMq zEuOoE5Kkkv 9ww3n5ARfkq hb5XsVTAfv0 NKugQfNEC64 hnBIDnFDLda vViozil9bGw 2QeETyHDI4W erPhRI8x6M0</t>
+  </si>
+  <si>
+    <t>vcW8z9OYcv</t>
+  </si>
+  <si>
+    <t>Source Action Auto2021-06-04T11:47:03.202</t>
+  </si>
+  <si>
+    <t>Type Action Auto 2021-06-04T11:47:12.073</t>
+  </si>
+  <si>
+    <t>désignation  action  simplifie  kxFpa6TusbH hVNMQ9Tz5sp RHhTnZ6fi93 bedOyXkPapt nyMNSiSZiQ9 NGmsYK7rlVp Z9uMwtYgUta jg8q7joQBWI U4tnYNS5ice 0q719qO9eXt mEoB3vwXBbP</t>
+  </si>
+  <si>
+    <t>LP2dmUn1HL</t>
   </si>
 </sst>
 </file>
@@ -1843,7 +1884,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -1953,9 +1994,6 @@
     <xf applyFill="1" applyFont="1" borderId="0" fillId="12" fontId="15" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="5" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Lien hypertexte" xfId="1"/>
@@ -2297,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,25 +2371,25 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>309</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="S2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="T2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row ht="14.45" r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="45"/>
       <c r="B3" s="35" t="s">
         <v>21</v>
@@ -2363,7 +2401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="25"/>
       <c r="B4" s="35" t="s">
         <v>24</v>
@@ -2474,19 +2512,19 @@
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="35" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="35" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C14" s="35"/>
       <c r="D14" s="35"/>
@@ -2494,13 +2532,13 @@
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="35" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -2614,7 +2652,7 @@
         <v>28</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="2" s="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
         <v>17</v>
       </c>
@@ -2634,7 +2672,7 @@
         <v>1000</v>
       </c>
       <c r="G2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="H2" s="56" t="s">
         <v>309</v>
@@ -2643,7 +2681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="3" s="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="56"/>
       <c r="B3" s="56"/>
       <c r="C3" s="56" t="s">
@@ -2659,14 +2697,14 @@
         <v>2000</v>
       </c>
       <c r="G3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="H3" s="56" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="I3" s="56"/>
     </row>
-    <row customFormat="1" r="4" s="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="56"/>
       <c r="B4" s="56" t="s">
         <v>18</v>
@@ -2691,7 +2729,7 @@
       </c>
       <c r="I4" s="56"/>
     </row>
-    <row customFormat="1" r="5" s="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="5" s="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="56" t="s">
         <v>17</v>
       </c>
@@ -2796,7 +2834,7 @@
     <col min="15" max="15" customWidth="true" width="38.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="15.75" r="1" s="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="15.75" r="1" s="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>15</v>
       </c>
@@ -2840,10 +2878,10 @@
         <v>26</v>
       </c>
       <c r="O1" s="37" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="29" spans="1:18" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row customFormat="1" ht="14.45" r="2" s="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>17</v>
       </c>
@@ -2851,10 +2889,10 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>494</v>
+        <v>503</v>
       </c>
       <c r="D2" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>40</v>
@@ -2863,10 +2901,10 @@
         <v>309</v>
       </c>
       <c r="G2" t="s">
-        <v>492</v>
+        <v>501</v>
       </c>
       <c r="H2" t="s">
-        <v>495</v>
+        <v>504</v>
       </c>
       <c r="I2" s="30" t="s">
         <v>47</v>
@@ -2878,26 +2916,26 @@
         <v>51</v>
       </c>
       <c r="L2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="M2" s="30"/>
       <c r="N2" s="30" t="s">
         <v>21</v>
       </c>
       <c r="O2" s="55" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="P2" s="55" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="Q2" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
       <c r="R2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row ht="14.45" r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>196</v>
       </c>
@@ -2941,7 +2979,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>17</v>
       </c>
@@ -2982,7 +3020,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>17</v>
       </c>
@@ -3026,7 +3064,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>17</v>
       </c>
@@ -3064,7 +3102,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>17</v>
       </c>
@@ -3105,7 +3143,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>17</v>
       </c>
@@ -3143,7 +3181,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>17</v>
       </c>
@@ -3250,7 +3288,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>119</v>
       </c>
@@ -3276,7 +3314,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>119</v>
       </c>
@@ -3340,7 +3378,7 @@
         <v>320</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="5" s="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>194</v>
       </c>
@@ -3425,7 +3463,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
         <v>278</v>
       </c>
@@ -3441,7 +3479,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="3" s="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>281</v>
       </c>
@@ -3456,7 +3494,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>278</v>
       </c>
@@ -3472,7 +3510,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>287</v>
       </c>
@@ -3531,7 +3569,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>131</v>
       </c>
@@ -3539,7 +3577,7 @@
         <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D2" s="35"/>
       <c r="E2" s="35"/>
@@ -3557,7 +3595,7 @@
       <c r="D3" s="35"/>
       <c r="E3" s="35"/>
     </row>
-    <row customFormat="1" r="4" s="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>131</v>
       </c>
@@ -3572,7 +3610,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="35"/>
       <c r="B5" s="35"/>
       <c r="D5" s="35"/>
@@ -4214,7 +4252,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>137</v>
       </c>
@@ -4222,13 +4260,13 @@
         <v>309</v>
       </c>
       <c r="C2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D2" s="35" t="s">
         <v>137</v>
       </c>
       <c r="E2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F2" s="35">
         <v>50</v>
@@ -4315,10 +4353,10 @@
     </row>
     <row customFormat="1" r="2" s="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>212</v>
@@ -4337,12 +4375,12 @@
       <c r="I2" s="25"/>
       <c r="J2" s="25"/>
     </row>
-    <row customFormat="1" r="3" s="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="3" s="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B3" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -4357,7 +4395,7 @@
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
     </row>
-    <row customFormat="1" r="4" s="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="24"/>
@@ -4381,7 +4419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="5" s="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="25"/>
       <c r="B5" s="25"/>
       <c r="C5" s="24"/>
@@ -4755,37 +4793,37 @@
   <sheetData>
     <row customFormat="1" ht="15.75" r="1" s="65" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B1" s="66" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C1" s="66" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E1" s="66" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="F1" s="66" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G1" s="66" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="I1" s="66" t="s">
         <v>129</v>
       </c>
       <c r="J1" s="66" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="K1" s="66" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="L1" s="66" t="s">
         <v>82</v>
@@ -4794,209 +4832,209 @@
         <v>239</v>
       </c>
       <c r="N1" s="66" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="O1" s="66" t="s">
         <v>240</v>
       </c>
       <c r="P1" s="66" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q1" s="66" t="s">
         <v>3</v>
       </c>
       <c r="R1" s="66" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="S1" s="66" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="T1" s="66" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="U1" s="66" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="V1" s="66" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="W1" s="66" t="s">
+        <v>398</v>
+      </c>
+      <c r="X1" s="66" t="s">
+        <v>399</v>
+      </c>
+      <c r="Y1" s="66" t="s">
+        <v>400</v>
+      </c>
+      <c r="Z1" s="66" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA1" s="66" t="s">
         <v>397</v>
       </c>
-      <c r="X1" s="66" t="s">
-        <v>398</v>
-      </c>
-      <c r="Y1" s="66" t="s">
-        <v>399</v>
-      </c>
-      <c r="Z1" s="66" t="s">
-        <v>400</v>
-      </c>
-      <c r="AA1" s="66" t="s">
-        <v>396</v>
-      </c>
       <c r="AB1" s="66" t="s">
+        <v>436</v>
+      </c>
+      <c r="AC1" s="66" t="s">
+        <v>402</v>
+      </c>
+      <c r="AD1" s="66" t="s">
+        <v>403</v>
+      </c>
+      <c r="AE1" s="66" t="s">
+        <v>404</v>
+      </c>
+      <c r="AF1" s="66" t="s">
+        <v>405</v>
+      </c>
+      <c r="AG1" s="66" t="s">
+        <v>406</v>
+      </c>
+      <c r="AH1" s="66" t="s">
+        <v>407</v>
+      </c>
+      <c r="AI1" s="66" t="s">
+        <v>408</v>
+      </c>
+      <c r="AJ1" s="66" t="s">
+        <v>409</v>
+      </c>
+      <c r="AK1" s="66" t="s">
+        <v>410</v>
+      </c>
+      <c r="AL1" s="66" t="s">
+        <v>411</v>
+      </c>
+      <c r="AM1" s="66" t="s">
+        <v>412</v>
+      </c>
+      <c r="AN1" s="66" t="s">
+        <v>413</v>
+      </c>
+      <c r="AO1" s="66" t="s">
+        <v>414</v>
+      </c>
+      <c r="AP1" s="66" t="s">
+        <v>415</v>
+      </c>
+      <c r="AQ1" s="66" t="s">
+        <v>416</v>
+      </c>
+      <c r="AR1" s="66" t="s">
+        <v>417</v>
+      </c>
+      <c r="AS1" s="65" t="s">
+        <v>434</v>
+      </c>
+      <c r="AT1" s="65" t="s">
         <v>435</v>
-      </c>
-      <c r="AC1" s="66" t="s">
-        <v>401</v>
-      </c>
-      <c r="AD1" s="66" t="s">
-        <v>402</v>
-      </c>
-      <c r="AE1" s="66" t="s">
-        <v>403</v>
-      </c>
-      <c r="AF1" s="66" t="s">
-        <v>404</v>
-      </c>
-      <c r="AG1" s="66" t="s">
-        <v>405</v>
-      </c>
-      <c r="AH1" s="66" t="s">
-        <v>406</v>
-      </c>
-      <c r="AI1" s="66" t="s">
-        <v>407</v>
-      </c>
-      <c r="AJ1" s="66" t="s">
-        <v>408</v>
-      </c>
-      <c r="AK1" s="66" t="s">
-        <v>409</v>
-      </c>
-      <c r="AL1" s="66" t="s">
-        <v>410</v>
-      </c>
-      <c r="AM1" s="66" t="s">
-        <v>411</v>
-      </c>
-      <c r="AN1" s="66" t="s">
-        <v>412</v>
-      </c>
-      <c r="AO1" s="66" t="s">
-        <v>413</v>
-      </c>
-      <c r="AP1" s="66" t="s">
-        <v>414</v>
-      </c>
-      <c r="AQ1" s="66" t="s">
-        <v>415</v>
-      </c>
-      <c r="AR1" s="66" t="s">
-        <v>416</v>
-      </c>
-      <c r="AS1" s="65" t="s">
-        <v>433</v>
-      </c>
-      <c r="AT1" s="65" t="s">
-        <v>434</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="12" r="2" s="68" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="I2" t="s">
         <v>131</v>
       </c>
       <c r="J2" s="68" t="s">
+        <v>422</v>
+      </c>
+      <c r="K2" s="68" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q2" s="68" t="s">
+        <v>424</v>
+      </c>
+      <c r="R2" s="67" t="s">
+        <v>425</v>
+      </c>
+      <c r="S2" t="s">
+        <v>426</v>
+      </c>
+      <c r="U2" t="s">
+        <v>460</v>
+      </c>
+      <c r="V2" t="s">
+        <v>458</v>
+      </c>
+      <c r="X2" t="s">
+        <v>419</v>
+      </c>
+      <c r="Z2" s="68" t="s">
+        <v>428</v>
+      </c>
+      <c r="AA2" s="68" t="s">
+        <v>427</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>457</v>
+      </c>
+      <c r="AC2" s="68" t="s">
+        <v>429</v>
+      </c>
+      <c r="AD2" s="67" t="s">
+        <v>430</v>
+      </c>
+      <c r="AF2" s="68" t="s">
         <v>421</v>
       </c>
-      <c r="K2" s="68" t="s">
-        <v>422</v>
-      </c>
-      <c r="Q2" s="68" t="s">
-        <v>423</v>
-      </c>
-      <c r="R2" s="67" t="s">
-        <v>424</v>
-      </c>
-      <c r="S2" t="s">
-        <v>425</v>
-      </c>
-      <c r="U2" t="s">
-        <v>459</v>
-      </c>
-      <c r="V2" t="s">
-        <v>457</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="AG2" s="68" t="s">
+        <v>431</v>
+      </c>
+      <c r="AI2" s="68" t="s">
+        <v>432</v>
+      </c>
+      <c r="AJ2" s="68" t="s">
         <v>418</v>
       </c>
-      <c r="Z2" s="68" t="s">
-        <v>427</v>
-      </c>
-      <c r="AA2" s="68" t="s">
-        <v>426</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>456</v>
-      </c>
-      <c r="AC2" s="68" t="s">
-        <v>428</v>
-      </c>
-      <c r="AD2" s="67" t="s">
-        <v>429</v>
-      </c>
-      <c r="AF2" s="68" t="s">
-        <v>420</v>
-      </c>
-      <c r="AG2" s="68" t="s">
-        <v>430</v>
-      </c>
-      <c r="AI2" s="68" t="s">
-        <v>431</v>
-      </c>
-      <c r="AJ2" s="68" t="s">
-        <v>417</v>
-      </c>
       <c r="AK2" s="68" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AL2" s="68" t="s">
         <v>212</v>
       </c>
       <c r="AN2" s="68" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AO2" s="68" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AQ2" s="68" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AT2" s="68" t="s">
         <v>309</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="61" spans="1:46" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="3" s="61" spans="1:46" x14ac:dyDescent="0.3">
       <c r="Y3" s="61">
         <v>24</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="61" spans="1:46" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="61" spans="1:46" x14ac:dyDescent="0.3">
       <c r="U4" s="61">
         <v>20</v>
       </c>
@@ -5050,9 +5088,9 @@
         <v>173</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="2" s="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>171</v>
@@ -5067,7 +5105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="3" s="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -5078,7 +5116,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row customFormat="1" r="4" s="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -5089,7 +5127,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row customFormat="1" r="5" s="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="5" s="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -5426,9 +5464,9 @@
         <v>170</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="2" s="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>171</v>
@@ -5446,7 +5484,7 @@
         <v>166</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="3" s="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -5458,7 +5496,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row customFormat="1" r="4" s="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -5470,7 +5508,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row customFormat="1" r="5" s="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="5" s="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -5760,7 +5798,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>17</v>
       </c>
@@ -5805,10 +5843,10 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q2" t="s">
         <v>472</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>471</v>
       </c>
       <c r="R2" s="30" t="s">
         <v>65</v>
@@ -5820,19 +5858,19 @@
         <v>303</v>
       </c>
       <c r="U2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="V2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="W2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="X2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row ht="14.45" r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>17</v>
       </c>
@@ -6132,7 +6170,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0" zoomScale="115">
-      <selection activeCell="G1" sqref="E1:G5"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6177,7 +6215,7 @@
         <v>25</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="2" s="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>176</v>
       </c>
@@ -6200,7 +6238,7 @@
         <v>309</v>
       </c>
       <c r="H2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="I2" s="35" t="s">
         <v>21</v>
@@ -6235,7 +6273,7 @@
         <v>207</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="35"/>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
@@ -6505,79 +6543,6 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5857249F-7E86-4117-9FB2-C8B986B62128}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="21.85546875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row ht="18.75" r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>505</v>
-      </c>
-      <c r="B1" t="s">
-        <v>506</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>499</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
-        <v>501</v>
-      </c>
-      <c r="B2" s="56" t="s">
-        <v>497</v>
-      </c>
-      <c r="C2" s="56" t="s">
-        <v>502</v>
-      </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -6623,7 +6588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>176</v>
       </c>
@@ -6643,7 +6608,7 @@
         <v>309</v>
       </c>
       <c r="G2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H2" s="30" t="s">
         <v>309</v>
@@ -6654,7 +6619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -6678,7 +6643,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>260</v>
       </c>
@@ -6689,7 +6654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>261</v>
       </c>
@@ -6700,7 +6665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>262</v>
       </c>
@@ -6711,7 +6676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>263</v>
       </c>
@@ -6856,7 +6821,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B18" s="62" t="s">
         <v>47</v>
@@ -6876,12 +6841,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="115">
-      <selection sqref="A1:D2"/>
+    <sheetView topLeftCell="P1" workbookViewId="0" zoomScale="115">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6906,63 +6871,63 @@
         <v>16</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
       <c r="K1" s="26" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="N1" s="26" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="O1" s="26" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P1" s="26" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="Q1" s="26" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="R1" s="26" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="S1" s="26" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="T1" s="26" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="U1" s="26" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="V1" s="26" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="W1" s="26"/>
       <c r="X1" s="26"/>
@@ -6976,7 +6941,7 @@
       <c r="AF1" s="26"/>
       <c r="AG1" s="26"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>18</v>
       </c>
@@ -6984,19 +6949,19 @@
         <v>17</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>189</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>24</v>
@@ -7004,28 +6969,28 @@
       <c r="I2" s="29"/>
       <c r="J2" s="29"/>
       <c r="K2" t="s">
+        <v>467</v>
+      </c>
+      <c r="L2" t="s">
         <v>466</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>468</v>
+      </c>
+      <c r="N2" t="s">
+        <v>441</v>
+      </c>
+      <c r="O2" t="s">
+        <v>464</v>
+      </c>
+      <c r="P2" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q2" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="R2" t="s">
         <v>465</v>
-      </c>
-      <c r="M2" t="s">
-        <v>467</v>
-      </c>
-      <c r="N2" t="s">
-        <v>440</v>
-      </c>
-      <c r="O2" t="s">
-        <v>463</v>
-      </c>
-      <c r="P2" t="s">
-        <v>441</v>
-      </c>
-      <c r="Q2" s="29" t="s">
-        <v>346</v>
-      </c>
-      <c r="R2" t="s">
-        <v>464</v>
       </c>
       <c r="S2" s="29">
         <v>1</v>
@@ -7051,9 +7016,9 @@
       <c r="AF2" s="29"/>
       <c r="AG2" s="29"/>
     </row>
-    <row customFormat="1" ht="18.75" r="4" s="26" spans="1:33" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="18" r="4" s="26" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row customFormat="1" r="5" s="29" spans="1:33" x14ac:dyDescent="0.25"/>
@@ -7062,7 +7027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:DZ2"/>
   <sheetViews>
@@ -7078,10 +7043,10 @@
   <sheetData>
     <row customFormat="1" r="1" s="58" spans="1:129" x14ac:dyDescent="0.3">
       <c r="A1" s="59" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C1" s="60"/>
       <c r="D1" s="60"/>
@@ -7211,12 +7176,12 @@
       <c r="DX1" s="60"/>
       <c r="DY1" s="60"/>
     </row>
-    <row r="2" spans="1:129" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:129" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -7225,12 +7190,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7242,16 +7207,16 @@
   <sheetData>
     <row customFormat="1" ht="18" r="1" s="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="64" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C1" s="64" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row ht="14.45" r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>260</v>
       </c>
@@ -7259,7 +7224,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>258</v>
       </c>
@@ -7267,7 +7232,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>263</v>
       </c>
@@ -7275,15 +7240,15 @@
         <v>309</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B5" s="61" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row ht="14.45" r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>264</v>
       </c>
@@ -7293,7 +7258,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B7" s="61" t="s">
         <v>309</v>
@@ -7376,7 +7341,7 @@
         <v>262</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7466,7 +7431,7 @@
         <v>24022</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="3" s="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -7477,7 +7442,7 @@
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
     </row>
-    <row customFormat="1" r="4" s="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="30"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -7488,7 +7453,7 @@
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
     </row>
-    <row customFormat="1" r="5" s="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="5" s="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
@@ -7597,7 +7562,7 @@
       </c>
       <c r="N1" s="61"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -7608,10 +7573,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="J2" s="61" t="s">
         <v>9</v>
@@ -7623,13 +7588,13 @@
         <v>10</v>
       </c>
       <c r="M2" s="61" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N2" s="61" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -7640,7 +7605,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E3" t="s">
         <v>312</v>
@@ -7765,22 +7730,22 @@
         <v>26</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="Y1" s="7" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="2" spans="1:25" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row customFormat="1" ht="14.45" r="2" s="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -7827,7 +7792,7 @@
         <v>75</v>
       </c>
       <c r="P2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="Q2" s="35" t="s">
         <v>309</v>
@@ -7842,7 +7807,7 @@
         <v>309</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="V2" s="2">
         <v>1000</v>
@@ -7851,13 +7816,13 @@
         <v>150</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="Y2" s="62">
         <v>30</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="3" s="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -8417,7 +8382,7 @@
         <v>55</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="2" s="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -8428,17 +8393,17 @@
         <v>309</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="3" s="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="5" s="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -8612,7 +8577,7 @@
         <v>55</v>
       </c>
       <c r="H1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>181</v>
@@ -8665,43 +8630,43 @@
     </row>
     <row customFormat="1" ht="18.75" r="2" s="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>481</v>
+        <v>517</v>
       </c>
       <c r="B2" t="s">
-        <v>482</v>
+        <v>518</v>
       </c>
       <c r="C2" t="s">
+        <v>485</v>
+      </c>
+      <c r="D2" t="s">
+        <v>486</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="H2" t="s">
+        <v>478</v>
+      </c>
+      <c r="I2" t="s">
+        <v>376</v>
+      </c>
+      <c r="J2" t="s">
         <v>484</v>
-      </c>
-      <c r="D2" t="s">
-        <v>485</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>309</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>309</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>309</v>
-      </c>
-      <c r="H2" t="s">
-        <v>477</v>
-      </c>
-      <c r="I2" t="s">
-        <v>375</v>
-      </c>
-      <c r="J2" t="s">
-        <v>483</v>
       </c>
       <c r="K2" s="31">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>486</v>
+        <v>519</v>
       </c>
       <c r="M2" t="s">
-        <v>487</v>
+        <v>520</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>17</v>
@@ -8719,22 +8684,22 @@
         <v>247</v>
       </c>
       <c r="S2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="T2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="U2" t="s">
         <v>191</v>
       </c>
       <c r="V2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="W2" t="s">
         <v>191</v>
       </c>
       <c r="X2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row customFormat="1" ht="18.75" r="3" s="26" spans="1:24" x14ac:dyDescent="0.3">
@@ -8760,10 +8725,10 @@
         <v>309</v>
       </c>
       <c r="H3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>246</v>
@@ -8772,7 +8737,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="M3" s="29" t="s">
         <v>256</v>
@@ -8793,7 +8758,7 @@
         <v>247</v>
       </c>
       <c r="S3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="T3" s="29" t="s">
         <v>253</v>
@@ -8811,7 +8776,7 @@
         <v>253</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="D4" s="31"/>
       <c r="H4" s="31"/>
       <c r="I4" s="31"/>
@@ -9374,7 +9339,7 @@
         <v>20</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="2" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>257</v>
       </c>
@@ -9416,7 +9381,7 @@
       </c>
       <c r="N2" s="30"/>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="3" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>257</v>
       </c>
@@ -9448,7 +9413,7 @@
       </c>
       <c r="N3" s="30"/>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>257</v>
       </c>
@@ -9484,7 +9449,7 @@
         <v>24</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="5" s="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>257</v>
       </c>
@@ -9877,22 +9842,22 @@
         <v>304</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="S1" s="57" t="s">
+        <v>360</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="U1" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="T1" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="30" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row customFormat="1" ht="14.45" r="2" s="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>17</v>
       </c>
@@ -9921,7 +9886,7 @@
         <v>108</v>
       </c>
       <c r="J2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="K2" s="30">
         <v>126</v>
@@ -9945,10 +9910,10 @@
         <v>12</v>
       </c>
       <c r="S2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="T2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="U2"/>
     </row>
@@ -9994,7 +9959,7 @@
         <v>309</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="14.45" r="4" s="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
verfication   d'ajout de  fiche   évaluation aspect
</commit_message>
<xml_diff>
--- a/resources/testData/TestData.xlsx
+++ b/resources/testData/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{330F5E6A-BDBB-4409-BF09-F10F1F0D34EE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{F39348D5-297D-4F3A-A39B-BBF33D0D9108}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="20" firstSheet="15" tabRatio="729" windowHeight="13140" windowWidth="24240" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="20" firstSheet="13" tabRatio="729" windowHeight="13140" windowWidth="24240" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Input" r:id="rId1" sheetId="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="505">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -1535,12 +1535,6 @@
     <t>rCwkHg69kz</t>
   </si>
   <si>
-    <t>http://10.66.245.30/Qualipro_saphir</t>
-  </si>
-  <si>
-    <t>sana</t>
-  </si>
-  <si>
     <t>2021-06-02T10:13:56.685749800</t>
   </si>
   <si>
@@ -1559,37 +1553,37 @@
     <t>ORGANISME AUTO2021-06-02T10:15:02.973214</t>
   </si>
   <si>
+    <t xml:space="preserve">Facteur AUTO </t>
+  </si>
+  <si>
+    <t>Activité/Service</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition AUTO </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://10.66.245.30/w232</t>
+  </si>
+  <si>
+    <t>AUTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facteur </t>
+  </si>
+  <si>
+    <t>Aspect AUTO</t>
+  </si>
+  <si>
     <t>Aspect</t>
   </si>
   <si>
-    <t xml:space="preserve">Facteur AUTO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facteur </t>
-  </si>
-  <si>
-    <t>Activité/Service</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            Aspect AUTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieu AUTO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition AUTO </t>
-  </si>
-  <si>
-    <t>2021-06-04T10:32:42.698874100</t>
-  </si>
-  <si>
-    <t>2021-06-04T11:28:56.958915200</t>
-  </si>
-  <si>
-    <t>2021-06-04T11:28:59.222325700</t>
+    <t>Num  fiche</t>
+  </si>
+  <si>
+    <t>325</t>
   </si>
 </sst>
 </file>
@@ -1843,7 +1837,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -1953,7 +1947,8 @@
     <xf applyFill="1" applyFont="1" borderId="0" fillId="12" fontId="15" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="5" fontId="1" numFmtId="0" xfId="0">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="10" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="6" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2298,7 +2293,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,16 +2328,16 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>309</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>489</v>
+        <v>499</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>489</v>
+        <v>499</v>
       </c>
       <c r="S2" t="s">
         <v>353</v>
@@ -2494,13 +2489,13 @@
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="35" t="s">
-        <v>489</v>
+        <v>316</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>489</v>
+        <v>316</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>489</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -2559,7 +2554,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink display="http://10.66.245.30/Qualipro_saphir" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2851,10 +2846,10 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>40</v>
@@ -2863,10 +2858,10 @@
         <v>309</v>
       </c>
       <c r="G2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="H2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I2" s="30" t="s">
         <v>47</v>
@@ -2891,10 +2886,10 @@
         <v>349</v>
       </c>
       <c r="Q2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="R2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -6506,9 +6501,11 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5857249F-7E86-4117-9FB2-C8B986B62128}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6517,63 +6514,74 @@
     <col min="3" max="3" customWidth="true" width="29.5703125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="22.42578125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.85546875" collapsed="false"/>
   </cols>
   <sheetData>
-    <row ht="18.75" r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>505</v>
-      </c>
-      <c r="B1" t="s">
-        <v>506</v>
-      </c>
-      <c r="C1" s="26" t="s">
+    <row customFormat="1" ht="18.75" r="1" s="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="69" t="s">
+        <v>502</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>499</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="21" t="s">
+        <v>495</v>
+      </c>
+      <c r="E1" s="70" t="s">
+        <v>496</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>501</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>502</v>
+        <v>175</v>
       </c>
       <c r="D2" s="56"/>
       <c r="E2" s="56" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+      <c r="F2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="36"/>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="35"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="35"/>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="35"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>